<commit_message>
Added thickness as an input. Changed flange hub for thicknesses over 0.88 inches
</commit_message>
<xml_diff>
--- a/1_in_bolt_Calculations.xlsx
+++ b/1_in_bolt_Calculations.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Bolting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c6dfa9304cd77db/Documents/Spring 2020/Flange Plugin/Flange_GUI/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_6BE3275633AF48FC5E3CCA863B540A435C979D60" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BFC6E1CB-FB8E-4F9E-B404-DF8E03A2DF75}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25860" windowHeight="11310"/>
+    <workbookView minimized="1" xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="18">
   <si>
     <t>Raised</t>
   </si>
@@ -59,9 +66,6 @@
     <t>Stress</t>
   </si>
   <si>
-    <t>Head</t>
-  </si>
-  <si>
     <t>(in.)</t>
   </si>
   <si>
@@ -75,12 +79,18 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Across Flat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -137,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -154,6 +164,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,7 +199,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Straight Connector 1"/>
+        <xdr:cNvPr id="2" name="Straight Connector 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -488,29 +505,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:Q16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X9" sqref="X9"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
+      <c r="K2" s="8" t="s">
+        <v>1</v>
+      </c>
       <c r="L2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
@@ -531,13 +551,13 @@
         <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
@@ -560,42 +580,42 @@
         <v>10</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C6" s="3">
         <v>6.25E-2</v>
       </c>
@@ -626,33 +646,33 @@
         <v>0.984375</v>
       </c>
     </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.35">
       <c r="E9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="L9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="P9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.35">
       <c r="E10" s="5">
         <f>-($C$6+$D$6+$E$6/2+$L$6)</f>
         <v>-2.9193750000000001</v>
@@ -686,13 +706,13 @@
         <v>8.4375</v>
       </c>
     </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:17" x14ac:dyDescent="0.35">
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
     </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:17" x14ac:dyDescent="0.35">
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="6">
@@ -714,7 +734,7 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
     </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:17" x14ac:dyDescent="0.35">
       <c r="E13" s="6">
         <f>AVERAGE(F10,F16)</f>
         <v>8.03125</v>
@@ -729,7 +749,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
     </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.35">
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -740,7 +760,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
     </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:17" x14ac:dyDescent="0.35">
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
@@ -751,7 +771,7 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
     </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:17" x14ac:dyDescent="0.35">
       <c r="E16" s="5">
         <f>-($C$6+$D$6+$E$6/2+$L$6)</f>
         <v>-2.9193750000000001</v>
@@ -771,6 +791,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>